<commit_message>
added initial condition for raia in table
</commit_message>
<xml_diff>
--- a/Benchmark-Models/benchmark_model_characteristics.xlsx
+++ b/Benchmark-Models/benchmark_model_characteristics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="0" windowWidth="25400" windowHeight="14520" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="2240" yWindow="-16580" windowWidth="25400" windowHeight="14520" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_characteristics" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="126">
   <si>
     <t>Model Name</t>
   </si>
@@ -463,7 +463,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -869,21 +868,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -913,13 +897,28 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="295">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -1407,11 +1406,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2140194776"/>
-        <c:axId val="2128977976"/>
+        <c:axId val="2095602280"/>
+        <c:axId val="2095602632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2140194776"/>
+        <c:axId val="2095602280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,7 +1453,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2128977976"/>
+        <c:crossAx val="2095602632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1462,7 +1461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128977976"/>
+        <c:axId val="2095602632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,7 +1547,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2140194776"/>
+        <c:crossAx val="2095602280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2043,11 +2042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2141053448"/>
-        <c:axId val="2141097288"/>
+        <c:axId val="2095648024"/>
+        <c:axId val="2095651032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2141053448"/>
+        <c:axId val="2095648024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2104,12 +2103,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141097288"/>
+        <c:crossAx val="2095651032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2141097288"/>
+        <c:axId val="2095651032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,7 +2165,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141053448"/>
+        <c:crossAx val="2095648024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2375,11 +2374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2092000664"/>
-        <c:axId val="2092001032"/>
+        <c:axId val="2090316360"/>
+        <c:axId val="2090325208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2092000664"/>
+        <c:axId val="2090316360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2471,12 +2470,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2092001032"/>
+        <c:crossAx val="2090325208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2092001032"/>
+        <c:axId val="2090325208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2569,7 +2568,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2092000664"/>
+        <c:crossAx val="2090316360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -4628,7 +4627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5844,36 +5843,36 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="27"/>
+    <col min="1" max="1" width="10.83203125" style="22"/>
     <col min="2" max="2" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6" style="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="3.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6" style="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="3.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="190.33203125" style="27" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="27"/>
+    <col min="3" max="3" width="7.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="3.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="3.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="190.33203125" style="22" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="32" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5886,86 +5885,86 @@
       <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="8" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="9" t="s">
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="11" t="s">
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="78">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="23" t="s">
         <v>104</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="S2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="U2" s="11"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
@@ -5974,48 +5973,48 @@
       <c r="B3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="13">
         <v>25</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="14">
         <v>20</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="15">
         <v>23</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="16">
         <v>542</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="17">
         <v>27</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="17">
         <v>74</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="17">
         <v>12</v>
       </c>
-      <c r="J3" s="22">
-        <f>G3+H3+I3</f>
+      <c r="J3" s="17">
+        <f t="shared" ref="J3:J22" si="0">G3+H3+I3</f>
         <v>113</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23" t="s">
+      <c r="K3" s="18"/>
+      <c r="L3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="24" t="s">
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25" t="s">
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="25"/>
-      <c r="U3" s="26" t="s">
+      <c r="T3" s="20"/>
+      <c r="U3" s="21" t="s">
         <v>89</v>
       </c>
     </row>
@@ -6026,48 +6025,48 @@
       <c r="B4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="13">
         <v>6</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="14">
         <v>4</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="15">
         <v>13</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="16">
         <v>85</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="17">
         <v>10</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="17">
         <v>2</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="17">
         <v>4</v>
       </c>
-      <c r="J4" s="22">
-        <f>G4+H4+I4</f>
+      <c r="J4" s="17">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23" t="s">
+      <c r="K4" s="18"/>
+      <c r="L4" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="24" t="s">
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25" t="s">
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="25"/>
-      <c r="U4" s="26" t="s">
+      <c r="T4" s="20"/>
+      <c r="U4" s="21" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6078,48 +6077,48 @@
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="13">
         <v>4</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="15">
         <v>19</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="16">
         <v>27132</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="17">
         <v>70</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="17">
         <v>0</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="17">
         <v>2</v>
       </c>
-      <c r="J5" s="22">
-        <f>G5+H5+I5</f>
+      <c r="J5" s="17">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23" t="s">
+      <c r="K5" s="18"/>
+      <c r="L5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24" t="s">
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25" t="s">
+      <c r="R5" s="20"/>
+      <c r="S5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T5" s="25"/>
-      <c r="U5" s="26" t="s">
+      <c r="T5" s="20"/>
+      <c r="U5" s="21" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6130,48 +6129,48 @@
       <c r="B6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="13">
         <v>8</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="14">
         <v>3</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="15">
         <v>1</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="16">
         <v>48</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="17">
         <v>6</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="17">
         <v>0</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="17">
         <v>3</v>
       </c>
-      <c r="J6" s="22">
-        <f>G6+H6+I6</f>
+      <c r="J6" s="17">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23" t="s">
+      <c r="K6" s="18"/>
+      <c r="L6" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24" t="s">
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25" t="s">
+      <c r="R6" s="20"/>
+      <c r="S6" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T6" s="25"/>
-      <c r="U6" s="26" t="s">
+      <c r="T6" s="20"/>
+      <c r="U6" s="21" t="s">
         <v>96</v>
       </c>
     </row>
@@ -6182,100 +6181,100 @@
       <c r="B7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="13">
         <v>9</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="14">
         <v>2</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="15">
         <v>8</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="16">
         <v>43</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="17">
         <v>14</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="17">
         <v>4</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="17">
         <v>4</v>
       </c>
-      <c r="J7" s="22">
-        <f>G7+H7+I7</f>
+      <c r="J7" s="17">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23" t="s">
+      <c r="K7" s="18"/>
+      <c r="L7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24" t="s">
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25" t="s">
+      <c r="Q7" s="19"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="U7" s="26" t="s">
+      <c r="U7" s="21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="24" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="13">
         <v>7</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="14">
         <v>6</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="15">
         <v>6</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="16">
         <v>77</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="17">
         <v>13</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="17">
         <v>0</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="17">
         <v>0</v>
       </c>
-      <c r="J8" s="22">
-        <f>G8+H8+I8</f>
+      <c r="J8" s="17">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="24" t="s">
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25" t="s">
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T8" s="25"/>
-      <c r="U8" s="26" t="s">
+      <c r="T8" s="20"/>
+      <c r="U8" s="21" t="s">
         <v>85</v>
       </c>
     </row>
@@ -6286,48 +6285,48 @@
       <c r="B9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="13">
         <v>500</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="14">
         <v>3</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="15">
         <v>4</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="16">
         <v>105</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="17">
         <v>188</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="17">
         <v>0</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="17">
         <v>3</v>
       </c>
-      <c r="J9" s="22">
-        <f>G9+H9+I9</f>
+      <c r="J9" s="17">
+        <f t="shared" si="0"/>
         <v>191</v>
       </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23" t="s">
+      <c r="K9" s="18"/>
+      <c r="L9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24" t="s">
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="25" t="s">
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="26" t="s">
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="21" t="s">
         <v>91</v>
       </c>
     </row>
@@ -6338,48 +6337,48 @@
       <c r="B10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="13">
         <v>5</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="14">
         <v>4</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="15">
         <v>1</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="16">
         <v>21</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="17">
         <v>12</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="17">
         <v>0</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="17">
         <v>4</v>
       </c>
-      <c r="J10" s="22">
-        <f>G10+H10+I10</f>
+      <c r="J10" s="17">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="24" t="s">
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="25" t="s">
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="26" t="s">
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -6390,48 +6389,48 @@
       <c r="B11" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="13">
         <v>6</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="14">
         <v>2</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="15">
         <v>3</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="16">
         <v>72</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="17">
         <v>12</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="17">
         <v>8</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="17">
         <v>2</v>
       </c>
-      <c r="J11" s="22">
-        <f>G11+H11+I11</f>
+      <c r="J11" s="17">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23" t="s">
+      <c r="K11" s="18"/>
+      <c r="L11" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24" t="s">
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25" t="s">
+      <c r="R11" s="20"/>
+      <c r="S11" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T11" s="25"/>
-      <c r="U11" s="26" t="s">
+      <c r="T11" s="20"/>
+      <c r="U11" s="21" t="s">
         <v>84</v>
       </c>
     </row>
@@ -6442,48 +6441,48 @@
       <c r="B12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="13">
         <v>9</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="14">
         <v>3</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="15">
         <v>6</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="16">
         <v>144</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="17">
         <v>19</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="17">
         <v>0</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="17">
         <v>3</v>
       </c>
-      <c r="J12" s="22">
-        <f>G12+H12+I12</f>
+      <c r="J12" s="17">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24" t="s">
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25" t="s">
+      <c r="R12" s="20"/>
+      <c r="S12" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T12" s="25"/>
-      <c r="U12" s="26" t="s">
+      <c r="T12" s="20"/>
+      <c r="U12" s="21" t="s">
         <v>83</v>
       </c>
     </row>
@@ -6494,48 +6493,48 @@
       <c r="B13" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="13">
         <v>9</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="14">
         <v>6</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="15">
         <v>5</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="16">
         <v>221</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="17">
         <v>9</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="17">
         <v>53</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="17">
         <v>0</v>
       </c>
-      <c r="J13" s="22">
-        <f>G13+H13+I13</f>
+      <c r="J13" s="17">
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="24" t="s">
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25" t="s">
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T13" s="25"/>
-      <c r="U13" s="26" t="s">
+      <c r="T13" s="20"/>
+      <c r="U13" s="21" t="s">
         <v>87</v>
       </c>
     </row>
@@ -6546,48 +6545,48 @@
       <c r="B14" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="13">
         <v>25</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="14">
         <v>4</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="15">
         <v>109</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="16">
         <v>713</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="17">
         <v>34</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="17">
         <v>9</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="17">
         <v>3</v>
       </c>
-      <c r="J14" s="22">
-        <f>G14+H14+I14</f>
+      <c r="J14" s="17">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23" t="s">
+      <c r="K14" s="18"/>
+      <c r="L14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24" t="s">
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25" t="s">
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="U14" s="26" t="s">
+      <c r="U14" s="21" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6598,48 +6597,48 @@
       <c r="B15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="13">
         <v>33</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="14">
         <v>43</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="15">
         <v>12</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="16">
         <v>1755</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="17">
         <v>72</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="17">
         <v>0</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="17">
         <v>12</v>
       </c>
-      <c r="J15" s="22">
-        <f>G15+H15+I15</f>
+      <c r="J15" s="17">
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23" t="s">
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25" t="s">
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T15" s="25"/>
-      <c r="U15" s="26" t="s">
+      <c r="T15" s="20"/>
+      <c r="U15" s="21" t="s">
         <v>101</v>
       </c>
     </row>
@@ -6650,48 +6649,48 @@
       <c r="B16" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="13">
         <v>23</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="14">
         <v>22</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="15">
         <v>62</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="16">
         <v>1141</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="17">
         <v>41</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="17">
         <v>135</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="17">
         <v>21</v>
       </c>
-      <c r="J16" s="22">
-        <f>G16+H16+I16</f>
+      <c r="J16" s="17">
+        <f t="shared" si="0"/>
         <v>197</v>
       </c>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23" t="s">
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24" t="s">
+      <c r="O16" s="19"/>
+      <c r="P16" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25" t="s">
+      <c r="Q16" s="19"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T16" s="25"/>
-      <c r="U16" s="26" t="s">
+      <c r="T16" s="20"/>
+      <c r="U16" s="21" t="s">
         <v>102</v>
       </c>
     </row>
@@ -6702,46 +6701,48 @@
       <c r="B17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="13">
         <v>14</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="14">
         <v>8</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="15">
         <v>4</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="16">
         <v>205</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="17">
         <v>18</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="17">
         <v>21</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="17">
         <v>0</v>
       </c>
-      <c r="J17" s="22">
-        <f>G17+H17+I17</f>
+      <c r="J17" s="17">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23" t="s">
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="N17" s="23"/>
-      <c r="O17" s="24" t="s">
+      <c r="N17" s="18"/>
+      <c r="O17" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="26" t="s">
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="T17" s="20"/>
+      <c r="U17" s="21" t="s">
         <v>100</v>
       </c>
     </row>
@@ -6752,48 +6753,48 @@
       <c r="B18" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="13">
         <v>11</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="14">
         <v>4</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="15">
         <v>7</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="16">
         <v>292</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="17">
         <v>13</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="17">
         <v>15</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="17">
         <v>2</v>
       </c>
-      <c r="J18" s="22">
-        <f>G18+H18+I18</f>
+      <c r="J18" s="17">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23" t="s">
+      <c r="K18" s="18"/>
+      <c r="L18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="24" t="s">
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25" t="s">
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T18" s="25"/>
-      <c r="U18" s="26" t="s">
+      <c r="T18" s="20"/>
+      <c r="U18" s="21" t="s">
         <v>92</v>
       </c>
     </row>
@@ -6804,48 +6805,48 @@
       <c r="B19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="13">
         <v>13</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="14">
         <v>11</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="15">
         <v>110</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="16">
         <v>2220</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="17">
         <v>23</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="17">
         <v>160</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="17">
         <v>86</v>
       </c>
-      <c r="J19" s="22">
-        <f>G19+H19+I19</f>
+      <c r="J19" s="17">
+        <f t="shared" si="0"/>
         <v>269</v>
       </c>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23" t="s">
+      <c r="K19" s="18"/>
+      <c r="L19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24" t="s">
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-      <c r="T19" s="25" t="s">
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="U19" s="26" t="s">
+      <c r="U19" s="21" t="s">
         <v>98</v>
       </c>
     </row>
@@ -6856,48 +6857,48 @@
       <c r="B20" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="13">
         <v>9</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="14">
         <v>3</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="15">
         <v>1</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="16">
         <v>46</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="17">
         <v>9</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="17">
         <v>2</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="17">
         <v>3</v>
       </c>
-      <c r="J20" s="22">
-        <f>G20+H20+I20</f>
+      <c r="J20" s="17">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24" t="s">
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25" t="s">
+      <c r="R20" s="20"/>
+      <c r="S20" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="T20" s="25"/>
-      <c r="U20" s="26" t="s">
+      <c r="T20" s="20"/>
+      <c r="U20" s="21" t="s">
         <v>88</v>
       </c>
     </row>
@@ -6908,48 +6909,48 @@
       <c r="B21" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="13">
         <v>7</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="14">
         <v>8</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="15">
         <v>3</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="16">
         <v>135</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="17">
         <v>26</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="17">
         <v>5</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="17">
         <v>5</v>
       </c>
-      <c r="J21" s="22">
-        <f>G21+H21+I21</f>
+      <c r="J21" s="17">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23" t="s">
+      <c r="K21" s="18"/>
+      <c r="L21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24" t="s">
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25" t="s">
+      <c r="Q21" s="19"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="U21" s="26" t="s">
+      <c r="U21" s="21" t="s">
         <v>94</v>
       </c>
     </row>
@@ -6960,48 +6961,48 @@
       <c r="B22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="13">
         <v>15</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="14">
         <v>15</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="15">
         <v>1</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="16">
         <v>60</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="17">
         <v>45</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="17">
         <v>0</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="17">
         <v>1</v>
       </c>
-      <c r="J22" s="22">
-        <f>G22+H22+I22</f>
+      <c r="J22" s="17">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23" t="s">
+      <c r="K22" s="18"/>
+      <c r="L22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24" t="s">
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="25" t="s">
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="U22" s="26" t="s">
+      <c r="U22" s="21" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last changes model characteristics
</commit_message>
<xml_diff>
--- a/Benchmark-Models/benchmark_model_characteristics.xlsx
+++ b/Benchmark-Models/benchmark_model_characteristics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43160" yWindow="-1920" windowWidth="20840" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="43160" yWindow="-1920" windowWidth="20840" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_characteristics" sheetId="1" r:id="rId1"/>
@@ -168,12 +168,6 @@
     <t>Non-Ident</t>
   </si>
   <si>
-    <t>Fixed errors</t>
-  </si>
-  <si>
-    <t>E0 from paper</t>
-  </si>
-  <si>
     <t>E1 from paper</t>
   </si>
   <si>
@@ -459,6 +453,12 @@
   </si>
   <si>
     <t>total overall</t>
+  </si>
+  <si>
+    <t>E3 from paper</t>
+  </si>
+  <si>
+    <t>Ex from paper</t>
   </si>
 </sst>
 </file>
@@ -1417,11 +1417,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="45982144"/>
-        <c:axId val="45984464"/>
+        <c:axId val="1963430464"/>
+        <c:axId val="1963432512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45982144"/>
+        <c:axId val="1963430464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45984464"/>
+        <c:crossAx val="1963432512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1472,7 +1472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45984464"/>
+        <c:axId val="1963432512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,7 +1579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45982144"/>
+        <c:crossAx val="1963430464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2095,11 +2095,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70478224"/>
-        <c:axId val="70480704"/>
+        <c:axId val="1963462096"/>
+        <c:axId val="1963464576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70478224"/>
+        <c:axId val="1963462096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,12 +2156,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70480704"/>
+        <c:crossAx val="1963464576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70480704"/>
+        <c:axId val="1963464576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,7 +2218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70478224"/>
+        <c:crossAx val="1963462096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2427,11 +2427,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="4532016"/>
-        <c:axId val="4255536"/>
+        <c:axId val="1963475920"/>
+        <c:axId val="1963479680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4532016"/>
+        <c:axId val="1963475920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2543,12 +2543,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4255536"/>
+        <c:crossAx val="1963479680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4255536"/>
+        <c:axId val="1963479680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2661,7 +2661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4532016"/>
+        <c:crossAx val="1963475920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -4730,8 +4730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4781,13 +4781,13 @@
         <v>32</v>
       </c>
       <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
       <c r="P1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -4798,7 +4798,7 @@
         <v>25</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>542</v>
@@ -4825,7 +4825,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -4879,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -4930,7 +4930,7 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -4984,7 +4984,7 @@
         <v>2</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -5035,7 +5035,7 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -5089,7 +5089,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -5236,7 +5236,7 @@
         <v>2</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -5287,7 +5287,7 @@
         <v>2</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -5317,7 +5317,7 @@
         <v>221</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F12">
         <v>49</v>
@@ -5338,7 +5338,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -5365,7 +5365,7 @@
         <v>25</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>713</v>
@@ -5392,7 +5392,7 @@
         <v>2</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -5443,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -5497,7 +5497,7 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -5551,7 +5551,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -5653,7 +5653,7 @@
         <v>2</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -5707,7 +5707,7 @@
         <v>2</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -5758,7 +5758,7 @@
         <v>1</v>
       </c>
       <c r="L20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -5812,7 +5812,7 @@
         <v>2</v>
       </c>
       <c r="L21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -5847,19 +5847,19 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -5867,19 +5867,19 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J26">
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -5887,19 +5887,19 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27">
         <v>2</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -5907,13 +5907,13 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="J28">
         <v>3</v>
       </c>
       <c r="K28" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -5927,11 +5927,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5993,84 +5993,84 @@
       <c r="Q1" s="26"/>
       <c r="R1" s="26"/>
       <c r="S1" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="T1" s="28"/>
       <c r="U1" s="28"/>
       <c r="V1" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
       <c r="G2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="R2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="10" t="s">
+      <c r="S2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" s="13">
         <v>25</v>
       </c>
       <c r="D3" s="14">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E3" s="15">
         <v>23</v>
@@ -6096,30 +6096,30 @@
       </c>
       <c r="L3" s="18"/>
       <c r="M3" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
       <c r="P3" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
       <c r="S3" s="20"/>
       <c r="T3" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U3" s="20"/>
       <c r="V3" s="21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="13">
         <v>6</v>
@@ -6151,30 +6151,30 @@
       </c>
       <c r="L4" s="18"/>
       <c r="M4" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
       <c r="P4" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="19"/>
       <c r="R4" s="19"/>
       <c r="S4" s="20"/>
       <c r="T4" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U4" s="20"/>
       <c r="V4" s="21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="13">
         <v>4</v>
@@ -6206,30 +6206,30 @@
       </c>
       <c r="L5" s="18"/>
       <c r="M5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
       <c r="R5" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S5" s="20"/>
       <c r="T5" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U5" s="20"/>
       <c r="V5" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="13">
         <v>8</v>
@@ -6261,30 +6261,30 @@
       </c>
       <c r="L6" s="18"/>
       <c r="M6" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
       <c r="R6" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S6" s="20"/>
       <c r="T6" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U6" s="20"/>
       <c r="V6" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C7" s="13">
         <v>9</v>
@@ -6316,30 +6316,30 @@
       </c>
       <c r="L7" s="18"/>
       <c r="M7" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R7" s="19"/>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
       <c r="U7" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V7" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C8" s="13">
         <v>7</v>
@@ -6370,31 +6370,31 @@
         <v>13</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
       <c r="P8" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="19"/>
       <c r="R8" s="19"/>
       <c r="S8" s="20"/>
       <c r="T8" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U8" s="20"/>
       <c r="V8" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" s="13">
         <v>500</v>
@@ -6426,30 +6426,30 @@
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
       <c r="P9" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q9" s="19"/>
       <c r="R9" s="19"/>
       <c r="S9" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>
       <c r="V9" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C10" s="13">
         <v>5</v>
@@ -6480,31 +6480,31 @@
         <v>12</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
       <c r="P10" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="19"/>
       <c r="R10" s="19"/>
       <c r="S10" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T10" s="20"/>
       <c r="U10" s="20"/>
       <c r="V10" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C11" s="13">
         <v>6</v>
@@ -6536,30 +6536,30 @@
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N11" s="18"/>
       <c r="O11" s="18"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S11" s="20"/>
       <c r="T11" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U11" s="20"/>
       <c r="V11" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C12" s="13">
         <v>9</v>
@@ -6590,7 +6590,7 @@
         <v>22</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
@@ -6598,23 +6598,23 @@
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S12" s="20"/>
       <c r="T12" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U12" s="20"/>
       <c r="V12" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C13" s="13">
         <v>9</v>
@@ -6623,7 +6623,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="15">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F13" s="16">
         <v>221</v>
@@ -6644,37 +6644,37 @@
         <v>78</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
       <c r="P13" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
       <c r="S13" s="20"/>
       <c r="T13" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U13" s="20"/>
       <c r="V13" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C14" s="13">
         <v>25</v>
       </c>
       <c r="D14" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" s="15">
         <v>109</v>
@@ -6700,30 +6700,30 @@
       </c>
       <c r="L14" s="18"/>
       <c r="M14" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S14" s="20"/>
       <c r="T14" s="20"/>
       <c r="U14" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V14" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C15" s="13">
         <v>33</v>
@@ -6757,28 +6757,28 @@
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="19"/>
       <c r="S15" s="20"/>
       <c r="T15" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U15" s="20"/>
       <c r="V15" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C16" s="13">
         <v>23</v>
@@ -6812,28 +6812,28 @@
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R16" s="19"/>
       <c r="S16" s="20"/>
       <c r="T16" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U16" s="20"/>
       <c r="V16" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C17" s="13">
         <v>14</v>
@@ -6866,29 +6866,29 @@
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O17" s="18"/>
       <c r="P17" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
       <c r="S17" s="20"/>
       <c r="T17" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U17" s="20"/>
       <c r="V17" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" s="13">
         <v>11</v>
@@ -6920,30 +6920,30 @@
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
       <c r="P18" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q18" s="19"/>
       <c r="R18" s="19"/>
       <c r="S18" s="20"/>
       <c r="T18" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U18" s="20"/>
       <c r="V18" s="21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" s="13">
         <v>13</v>
@@ -6974,30 +6974,30 @@
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
       <c r="R19" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S19" s="20"/>
       <c r="T19" s="20"/>
       <c r="U19" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V19" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C20" s="13">
         <v>9</v>
@@ -7028,7 +7028,7 @@
         <v>17</v>
       </c>
       <c r="L20" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
@@ -7036,23 +7036,23 @@
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
       <c r="R20" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S20" s="20"/>
       <c r="T20" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U20" s="20"/>
       <c r="V20" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C21" s="13">
         <v>7</v>
@@ -7084,30 +7084,30 @@
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
       <c r="P21" s="19"/>
       <c r="Q21" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R21" s="19"/>
       <c r="S21" s="20"/>
       <c r="T21" s="20"/>
       <c r="U21" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V21" s="21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" s="13">
         <v>15</v>
@@ -7139,22 +7139,22 @@
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
       <c r="R22" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S22" s="20"/>
       <c r="T22" s="20"/>
       <c r="U22" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V22" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction fujita, swameye nr parameters
</commit_message>
<xml_diff>
--- a/Benchmark-Models/benchmark_model_characteristics.xlsx
+++ b/Benchmark-Models/benchmark_model_characteristics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43160" yWindow="-1920" windowWidth="20840" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4760" yWindow="460" windowWidth="20840" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="model_characteristics" sheetId="1" r:id="rId1"/>
@@ -1417,11 +1417,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1963430464"/>
-        <c:axId val="1963432512"/>
+        <c:axId val="220590048"/>
+        <c:axId val="220591824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1963430464"/>
+        <c:axId val="220590048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963432512"/>
+        <c:crossAx val="220591824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1472,7 +1472,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1963432512"/>
+        <c:axId val="220591824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,7 +1579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963430464"/>
+        <c:crossAx val="220590048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1984,7 +1984,7 @@
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>49.0</c:v>
@@ -2008,7 +2008,7 @@
                   <c:v>260.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>36.0</c:v>
@@ -2095,11 +2095,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1963462096"/>
-        <c:axId val="1963464576"/>
+        <c:axId val="219678992"/>
+        <c:axId val="219681312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1963462096"/>
+        <c:axId val="219678992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,12 +2156,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963464576"/>
+        <c:crossAx val="219681312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1963464576"/>
+        <c:axId val="219681312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,7 +2218,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963462096"/>
+        <c:crossAx val="219678992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2346,7 +2346,7 @@
                   <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>49.0</c:v>
@@ -2370,7 +2370,7 @@
                   <c:v>260.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>36.0</c:v>
@@ -2427,11 +2427,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1963475920"/>
-        <c:axId val="1963479680"/>
+        <c:axId val="220628096"/>
+        <c:axId val="220631856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1963475920"/>
+        <c:axId val="220628096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2543,12 +2543,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963479680"/>
+        <c:crossAx val="220631856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1963479680"/>
+        <c:axId val="220631856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2661,7 +2661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1963475920"/>
+        <c:crossAx val="220628096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -4730,8 +4730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5269,7 +5269,7 @@
         <v>6</v>
       </c>
       <c r="F11">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G11">
         <v>19</v>
@@ -5278,7 +5278,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -5300,7 +5300,7 @@
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
-        <v>0.15277777777777779</v>
+        <v>0.13194444444444445</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -5689,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G19">
         <v>9</v>
@@ -5698,7 +5698,7 @@
         <v>4</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -5720,7 +5720,7 @@
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
-        <v>0.34782608695652173</v>
+        <v>0.28260869565217389</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -5927,11 +5927,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6580,11 +6580,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J12" s="17">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K12" s="17">
         <v>22</v>
@@ -7018,11 +7017,10 @@
         <v>4</v>
       </c>
       <c r="I20" s="17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J20" s="17">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K20" s="17">
         <v>17</v>

</xml_diff>